<commit_message>
updated model loading code logics
</commit_message>
<xml_diff>
--- a/jkfenner_image_process/machine_learning/hose_single/structure_data.xlsx
+++ b/jkfenner_image_process/machine_learning/hose_single/structure_data.xlsx
@@ -3439,7 +3439,7 @@
     <t xml:space="preserve">51534-67372</t>
   </si>
   <si>
-    <t xml:space="preserve">25412 1M400</t>
+    <t xml:space="preserve">254121M400</t>
   </si>
   <si>
     <t xml:space="preserve">C88398</t>
@@ -3886,7 +3886,7 @@
     <t xml:space="preserve">AP546</t>
   </si>
   <si>
-    <t xml:space="preserve">AP142 - 042</t>
+    <t xml:space="preserve">AP142-042</t>
   </si>
   <si>
     <t xml:space="preserve">AP1763</t>
@@ -3901,7 +3901,7 @@
     <t xml:space="preserve">AP1766A</t>
   </si>
   <si>
-    <t xml:space="preserve">AP1764A - 1734A</t>
+    <t xml:space="preserve">AP1764A-1734A</t>
   </si>
   <si>
     <t xml:space="preserve">AP8735</t>
@@ -4697,11 +4697,11 @@
   </sheetPr>
   <dimension ref="A1:G1682"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A940" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G956" activeCellId="0" sqref="G956"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1648" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1658" activeCellId="0" sqref="F1658"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="7.74"/>

</xml_diff>